<commit_message>
scenario dependent tables revised, hydrogen grid added, mandatory renewable heating for new buildings
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Scenario_HeatingSystem_MinimumRenewablePercentage.xlsx
+++ b/projects/test_building/input/Scenario_HeatingSystem_MinimumRenewablePercentage.xlsx
@@ -1,32 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RenderNew\projects\test_building\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/RenderNew/projects/test_building/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02AC814C-EA45-6C49-A8FC-6B4BC27A1DD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9135" yWindow="-17505" windowWidth="23955" windowHeight="16500" tabRatio="500"/>
+    <workbookView xWindow="9140" yWindow="-17500" windowWidth="23960" windowHeight="16500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -35,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
   <si>
     <t>id_region</t>
   </si>
@@ -173,12 +163,15 @@
   </si>
   <si>
     <t>fraction</t>
+  </si>
+  <si>
+    <t>id_scenario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -244,12 +237,12 @@
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Pivot Table Category" xfId="4"/>
-    <cellStyle name="Pivot Table Corner" xfId="1"/>
-    <cellStyle name="Pivot Table Field" xfId="3"/>
-    <cellStyle name="Pivot Table Result" xfId="6"/>
-    <cellStyle name="Pivot Table Title" xfId="5"/>
-    <cellStyle name="Pivot Table Value" xfId="2"/>
+    <cellStyle name="Pivot Table Category" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Pivot Table Corner" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Pivot Table Field" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Pivot Table Result" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Pivot Table Title" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Pivot Table Value" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -269,54 +262,55 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AS18" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:AS18"/>
-  <tableColumns count="45">
-    <tableColumn id="1" name="id_region"/>
-    <tableColumn id="2" name="id_sector"/>
-    <tableColumn id="3" name="id_subsector"/>
-    <tableColumn id="5" name="unit"/>
-    <tableColumn id="6" name="2010"/>
-    <tableColumn id="7" name="2011"/>
-    <tableColumn id="8" name="2012"/>
-    <tableColumn id="9" name="2013"/>
-    <tableColumn id="10" name="2014"/>
-    <tableColumn id="11" name="2015"/>
-    <tableColumn id="12" name="2016"/>
-    <tableColumn id="13" name="2017"/>
-    <tableColumn id="14" name="2018"/>
-    <tableColumn id="15" name="2019"/>
-    <tableColumn id="16" name="2020"/>
-    <tableColumn id="17" name="2021"/>
-    <tableColumn id="18" name="2022"/>
-    <tableColumn id="19" name="2023"/>
-    <tableColumn id="20" name="2024"/>
-    <tableColumn id="21" name="2025"/>
-    <tableColumn id="22" name="2026"/>
-    <tableColumn id="23" name="2027"/>
-    <tableColumn id="24" name="2028"/>
-    <tableColumn id="25" name="2029"/>
-    <tableColumn id="26" name="2030"/>
-    <tableColumn id="27" name="2031"/>
-    <tableColumn id="28" name="2032"/>
-    <tableColumn id="29" name="2033"/>
-    <tableColumn id="30" name="2034"/>
-    <tableColumn id="31" name="2035"/>
-    <tableColumn id="32" name="2036"/>
-    <tableColumn id="33" name="2037"/>
-    <tableColumn id="34" name="2038"/>
-    <tableColumn id="35" name="2039"/>
-    <tableColumn id="36" name="2040"/>
-    <tableColumn id="37" name="2041"/>
-    <tableColumn id="38" name="2042"/>
-    <tableColumn id="39" name="2043"/>
-    <tableColumn id="40" name="2044"/>
-    <tableColumn id="41" name="2045"/>
-    <tableColumn id="42" name="2046"/>
-    <tableColumn id="43" name="2047"/>
-    <tableColumn id="44" name="2048"/>
-    <tableColumn id="45" name="2049"/>
-    <tableColumn id="46" name="2050"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AT18" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:AT18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="46">
+    <tableColumn id="4" xr3:uid="{72136E91-1AE0-2743-BC88-8697ED68A2FE}" name="id_scenario"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id_region"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="id_sector"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="id_subsector"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="unit"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="2010"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="2011"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="2012"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="2013"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="2014"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="2015"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="2016"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="2017"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="2018"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="2019"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="2020"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="2021"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="2022"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="2023"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="2024"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="2025"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="2026"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="2027"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="2028"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="2029"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="2030"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="2031"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="2032"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="2033"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="2034"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="2035"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="2036"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="2037"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="2038"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="2039"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="2040"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="2041"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="2042"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="2043"/>
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="2044"/>
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="2045"/>
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="2046"/>
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="2047"/>
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="2048"/>
+    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="2049"/>
+    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="2050"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -618,171 +612,174 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AT18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:AS18"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>9</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>6</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>61</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>45</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
       <c r="F2">
         <v>0</v>
       </c>
@@ -823,7 +820,7 @@
         <v>0</v>
       </c>
       <c r="S2">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="T2">
         <v>0.65</v>
@@ -903,23 +900,26 @@
       <c r="AS2">
         <v>0.65</v>
       </c>
+      <c r="AT2">
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>9</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>31</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>45</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
       <c r="F3">
         <v>0</v>
       </c>
@@ -960,7 +960,7 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="T3">
         <v>0.65</v>
@@ -1040,23 +1040,26 @@
       <c r="AS3">
         <v>0.65</v>
       </c>
+      <c r="AT3">
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
         <v>9</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>32</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>45</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
       <c r="F4">
         <v>0</v>
       </c>
@@ -1097,7 +1100,7 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="T4">
         <v>0.65</v>
@@ -1177,23 +1180,26 @@
       <c r="AS4">
         <v>0.65</v>
       </c>
+      <c r="AT4">
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
         <v>9</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>33</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>45</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
       <c r="F5">
         <v>0</v>
       </c>
@@ -1234,7 +1240,7 @@
         <v>0</v>
       </c>
       <c r="S5">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="T5">
         <v>0.65</v>
@@ -1314,23 +1320,26 @@
       <c r="AS5">
         <v>0.65</v>
       </c>
+      <c r="AT5">
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
         <v>9</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>3</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>34</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>45</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
       <c r="F6">
         <v>0</v>
       </c>
@@ -1371,7 +1380,7 @@
         <v>0</v>
       </c>
       <c r="S6">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="T6">
         <v>0.65</v>
@@ -1451,23 +1460,26 @@
       <c r="AS6">
         <v>0.65</v>
       </c>
+      <c r="AT6">
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
         <v>9</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>3</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>35</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>45</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
       <c r="F7">
         <v>0</v>
       </c>
@@ -1508,7 +1520,7 @@
         <v>0</v>
       </c>
       <c r="S7">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="T7">
         <v>0.65</v>
@@ -1588,23 +1600,26 @@
       <c r="AS7">
         <v>0.65</v>
       </c>
+      <c r="AT7">
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>3</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>36</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>45</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
       <c r="F8">
         <v>0</v>
       </c>
@@ -1645,7 +1660,7 @@
         <v>0</v>
       </c>
       <c r="S8">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="T8">
         <v>0.65</v>
@@ -1725,23 +1740,26 @@
       <c r="AS8">
         <v>0.65</v>
       </c>
+      <c r="AT8">
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
         <v>9</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>3</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>37</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>45</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
       <c r="F9">
         <v>0</v>
       </c>
@@ -1782,7 +1800,7 @@
         <v>0</v>
       </c>
       <c r="S9">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="T9">
         <v>0.65</v>
@@ -1862,23 +1880,26 @@
       <c r="AS9">
         <v>0.65</v>
       </c>
+      <c r="AT9">
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>3</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>38</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>45</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
       <c r="F10">
         <v>0</v>
       </c>
@@ -1919,7 +1940,7 @@
         <v>0</v>
       </c>
       <c r="S10">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="T10">
         <v>0.65</v>
@@ -1999,23 +2020,26 @@
       <c r="AS10">
         <v>0.65</v>
       </c>
+      <c r="AT10">
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>3</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>39</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>45</v>
       </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
       <c r="F11">
         <v>0</v>
       </c>
@@ -2056,7 +2080,7 @@
         <v>0</v>
       </c>
       <c r="S11">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="T11">
         <v>0.65</v>
@@ -2136,23 +2160,26 @@
       <c r="AS11">
         <v>0.65</v>
       </c>
+      <c r="AT11">
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
         <v>9</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>3</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>310</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>45</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
       <c r="F12">
         <v>0</v>
       </c>
@@ -2193,7 +2220,7 @@
         <v>0</v>
       </c>
       <c r="S12">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="T12">
         <v>0.65</v>
@@ -2273,23 +2300,26 @@
       <c r="AS12">
         <v>0.65</v>
       </c>
+      <c r="AT12">
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
         <v>9</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>3</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>311</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>45</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
       <c r="F13">
         <v>0</v>
       </c>
@@ -2330,7 +2360,7 @@
         <v>0</v>
       </c>
       <c r="S13">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="T13">
         <v>0.65</v>
@@ -2410,23 +2440,26 @@
       <c r="AS13">
         <v>0.65</v>
       </c>
+      <c r="AT13">
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
         <v>9</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>3</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>312</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>45</v>
       </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
       <c r="F14">
         <v>0</v>
       </c>
@@ -2467,7 +2500,7 @@
         <v>0</v>
       </c>
       <c r="S14">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="T14">
         <v>0.65</v>
@@ -2547,23 +2580,26 @@
       <c r="AS14">
         <v>0.65</v>
       </c>
+      <c r="AT14">
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
         <v>9</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>3</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>313</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>45</v>
       </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
       <c r="F15">
         <v>0</v>
       </c>
@@ -2604,7 +2640,7 @@
         <v>0</v>
       </c>
       <c r="S15">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="T15">
         <v>0.65</v>
@@ -2684,23 +2720,26 @@
       <c r="AS15">
         <v>0.65</v>
       </c>
+      <c r="AT15">
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
         <v>9</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>3</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>314</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>45</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
       <c r="F16">
         <v>0</v>
       </c>
@@ -2741,7 +2780,7 @@
         <v>0</v>
       </c>
       <c r="S16">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="T16">
         <v>0.65</v>
@@ -2821,23 +2860,26 @@
       <c r="AS16">
         <v>0.65</v>
       </c>
+      <c r="AT16">
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
         <v>9</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>3</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>315</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>45</v>
       </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
       <c r="F17">
         <v>0</v>
       </c>
@@ -2878,7 +2920,7 @@
         <v>0</v>
       </c>
       <c r="S17">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="T17">
         <v>0.65</v>
@@ -2958,23 +3000,26 @@
       <c r="AS17">
         <v>0.65</v>
       </c>
+      <c r="AT17">
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
         <v>9</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>3</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>316</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>45</v>
       </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
       <c r="F18">
         <v>0</v>
       </c>
@@ -3015,7 +3060,7 @@
         <v>0</v>
       </c>
       <c r="S18">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="T18">
         <v>0.65</v>
@@ -3093,6 +3138,9 @@
         <v>0.65</v>
       </c>
       <c r="AS18">
+        <v>0.65</v>
+      </c>
+      <c r="AT18">
         <v>0.65</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- design of scenario-specific developments - calibration of person number for population
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Scenario_HeatingSystem_MinimumRenewablePercentage.xlsx
+++ b/projects/test_building/input/Scenario_HeatingSystem_MinimumRenewablePercentage.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RenderNew\projects\test_building\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace_sia\RenderNew\projects\test_building\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="note" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="51">
   <si>
     <t>id_region</t>
   </si>
@@ -165,6 +166,18 @@
   </si>
   <si>
     <t>id_scenario</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>65% renewable heating after 2024 (GEG)</t>
+  </si>
+  <si>
+    <t>65% renewable heating after 2030 (late implementation of GEG)</t>
+  </si>
+  <si>
+    <t>65% renewable heating after 2035 (late implementation of GEG)</t>
   </si>
 </sst>
 </file>
@@ -614,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="V38" sqref="V38"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19:AT35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3205,82 +3218,82 @@
         <v>0.65</v>
       </c>
       <c r="U19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="V19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="W19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="X19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Y19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Z19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AA19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AB19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AC19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AD19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AE19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AF19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AG19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AH19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AI19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AJ19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AK19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AL19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AM19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AN19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AO19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AP19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AQ19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AR19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AS19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AT19">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="20" spans="1:46" x14ac:dyDescent="0.25">
@@ -3345,82 +3358,82 @@
         <v>0.65</v>
       </c>
       <c r="U20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="V20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="W20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="X20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Y20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Z20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AA20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AB20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AC20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AD20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AE20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AF20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AG20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AH20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AI20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AJ20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AK20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AL20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AM20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AN20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AO20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AP20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AQ20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AR20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AS20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AT20">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="21" spans="1:46" x14ac:dyDescent="0.25">
@@ -3485,82 +3498,82 @@
         <v>0.65</v>
       </c>
       <c r="U21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="V21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="W21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="X21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Y21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Z21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AA21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AB21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AC21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AD21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AE21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AF21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AG21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AH21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AI21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AJ21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AK21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AL21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AM21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AN21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AO21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AP21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AQ21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AR21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AS21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AT21">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="22" spans="1:46" x14ac:dyDescent="0.25">
@@ -3625,82 +3638,82 @@
         <v>0.65</v>
       </c>
       <c r="U22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="V22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="W22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="X22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Y22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Z22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AA22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AB22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AC22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AD22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AE22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AF22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AG22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AH22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AI22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AJ22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AK22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AL22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AM22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AN22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AO22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AP22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AQ22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AR22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AS22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AT22">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="23" spans="1:46" x14ac:dyDescent="0.25">
@@ -3765,82 +3778,82 @@
         <v>0.65</v>
       </c>
       <c r="U23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="V23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="W23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="X23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Y23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Z23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AA23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AB23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AC23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AD23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AE23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AF23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AG23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AH23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AI23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AJ23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AK23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AL23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AM23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AN23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AO23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AP23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AQ23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AR23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AS23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AT23">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="24" spans="1:46" x14ac:dyDescent="0.25">
@@ -3905,82 +3918,82 @@
         <v>0.65</v>
       </c>
       <c r="U24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="V24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="W24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="X24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Y24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Z24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AA24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AB24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AC24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AD24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AE24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AF24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AG24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AH24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AI24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AJ24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AK24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AL24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AM24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AN24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AO24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AP24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AQ24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AR24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AS24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AT24">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="25" spans="1:46" x14ac:dyDescent="0.25">
@@ -4045,82 +4058,82 @@
         <v>0.65</v>
       </c>
       <c r="U25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="V25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="W25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="X25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Y25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Z25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AA25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AB25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AC25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AD25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AE25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AF25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AG25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AH25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AI25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AJ25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AK25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AL25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AM25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AN25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AO25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AP25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AQ25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AR25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AS25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AT25">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="26" spans="1:46" x14ac:dyDescent="0.25">
@@ -4185,82 +4198,82 @@
         <v>0.65</v>
       </c>
       <c r="U26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="V26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="W26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="X26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Y26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Z26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AA26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AB26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AC26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AD26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AE26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AF26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AG26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AH26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AI26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AJ26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AK26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AL26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AM26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AN26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AO26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AP26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AQ26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AR26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AS26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AT26">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="27" spans="1:46" x14ac:dyDescent="0.25">
@@ -4325,82 +4338,82 @@
         <v>0.65</v>
       </c>
       <c r="U27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="V27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="W27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="X27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Y27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Z27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AA27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AB27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AC27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AD27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AE27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AF27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AG27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AH27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AI27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AJ27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AK27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AL27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AM27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AN27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AO27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AP27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AQ27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AR27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AS27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AT27">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="28" spans="1:46" x14ac:dyDescent="0.25">
@@ -4465,82 +4478,82 @@
         <v>0.65</v>
       </c>
       <c r="U28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="V28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="W28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="X28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Y28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Z28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AA28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AB28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AC28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AD28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AE28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AF28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AG28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AH28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AI28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AJ28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AK28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AL28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AM28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AN28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AO28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AP28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AQ28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AR28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AS28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AT28">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="29" spans="1:46" x14ac:dyDescent="0.25">
@@ -4605,82 +4618,82 @@
         <v>0.65</v>
       </c>
       <c r="U29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="V29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="W29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="X29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Y29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Z29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AA29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AB29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AC29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AD29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AE29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AF29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AG29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AH29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AI29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AJ29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AK29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AL29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AM29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AN29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AO29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AP29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AQ29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AR29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AS29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AT29">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="30" spans="1:46" x14ac:dyDescent="0.25">
@@ -4745,82 +4758,82 @@
         <v>0.65</v>
       </c>
       <c r="U30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="V30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="W30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="X30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Y30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Z30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AA30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AB30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AC30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AD30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AE30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AF30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AG30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AH30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AI30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AJ30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AK30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AL30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AM30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AN30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AO30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AP30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AQ30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AR30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AS30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AT30">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="31" spans="1:46" x14ac:dyDescent="0.25">
@@ -4885,82 +4898,82 @@
         <v>0.65</v>
       </c>
       <c r="U31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="V31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="W31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="X31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Y31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Z31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AA31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AB31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AC31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AD31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AE31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AF31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AG31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AH31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AI31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AJ31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AK31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AL31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AM31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AN31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AO31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AP31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AQ31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AR31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AS31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AT31">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="32" spans="1:46" x14ac:dyDescent="0.25">
@@ -5025,82 +5038,82 @@
         <v>0.65</v>
       </c>
       <c r="U32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="V32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="W32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="X32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Y32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Z32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AA32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AB32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AC32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AD32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AE32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AF32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AG32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AH32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AI32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AJ32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AK32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AL32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AM32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AN32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AO32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AP32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AQ32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AR32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AS32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AT32">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="33" spans="1:46" x14ac:dyDescent="0.25">
@@ -5165,82 +5178,82 @@
         <v>0.65</v>
       </c>
       <c r="U33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="V33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="W33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="X33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Y33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Z33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AA33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AB33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AC33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AD33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AE33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AF33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AG33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AH33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AI33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AJ33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AK33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AL33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AM33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AN33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AO33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AP33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AQ33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AR33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AS33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AT33">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="34" spans="1:46" x14ac:dyDescent="0.25">
@@ -5305,82 +5318,82 @@
         <v>0.65</v>
       </c>
       <c r="U34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="V34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="W34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="X34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Y34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Z34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AA34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AB34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AC34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AD34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AE34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AF34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AG34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AH34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AI34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AJ34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AK34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AL34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AM34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AN34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AO34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AP34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AQ34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AR34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AS34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AT34">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="35" spans="1:46" x14ac:dyDescent="0.25">
@@ -5445,82 +5458,82 @@
         <v>0.65</v>
       </c>
       <c r="U35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="V35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="W35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="X35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Y35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="Z35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AA35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AB35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AC35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AD35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AE35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AF35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AG35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AH35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AI35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AJ35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AK35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AL35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AM35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AN35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AO35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AP35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AQ35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AR35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AS35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
       <c r="AT35">
-        <v>0.8</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="36" spans="1:46" x14ac:dyDescent="0.25">
@@ -5582,22 +5595,22 @@
         <v>0</v>
       </c>
       <c r="T36">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U36">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V36">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W36">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X36">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y36">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z36">
         <v>0.65</v>
@@ -5722,22 +5735,22 @@
         <v>0</v>
       </c>
       <c r="T37">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U37">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V37">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W37">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X37">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y37">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z37">
         <v>0.65</v>
@@ -5862,22 +5875,22 @@
         <v>0</v>
       </c>
       <c r="T38">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U38">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V38">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W38">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X38">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y38">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z38">
         <v>0.65</v>
@@ -6002,22 +6015,22 @@
         <v>0</v>
       </c>
       <c r="T39">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U39">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V39">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W39">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X39">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y39">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z39">
         <v>0.65</v>
@@ -6142,22 +6155,22 @@
         <v>0</v>
       </c>
       <c r="T40">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U40">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V40">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W40">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X40">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y40">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z40">
         <v>0.65</v>
@@ -6282,22 +6295,22 @@
         <v>0</v>
       </c>
       <c r="T41">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U41">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V41">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W41">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X41">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y41">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z41">
         <v>0.65</v>
@@ -6422,22 +6435,22 @@
         <v>0</v>
       </c>
       <c r="T42">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U42">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V42">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W42">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X42">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y42">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z42">
         <v>0.65</v>
@@ -6562,22 +6575,22 @@
         <v>0</v>
       </c>
       <c r="T43">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U43">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V43">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W43">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X43">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y43">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z43">
         <v>0.65</v>
@@ -6702,22 +6715,22 @@
         <v>0</v>
       </c>
       <c r="T44">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U44">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V44">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W44">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X44">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y44">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z44">
         <v>0.65</v>
@@ -6842,22 +6855,22 @@
         <v>0</v>
       </c>
       <c r="T45">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U45">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V45">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W45">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X45">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y45">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z45">
         <v>0.65</v>
@@ -6982,22 +6995,22 @@
         <v>0</v>
       </c>
       <c r="T46">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U46">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V46">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W46">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X46">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y46">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z46">
         <v>0.65</v>
@@ -7122,22 +7135,22 @@
         <v>0</v>
       </c>
       <c r="T47">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U47">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V47">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W47">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X47">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y47">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z47">
         <v>0.65</v>
@@ -7262,22 +7275,22 @@
         <v>0</v>
       </c>
       <c r="T48">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U48">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V48">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W48">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X48">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y48">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z48">
         <v>0.65</v>
@@ -7402,22 +7415,22 @@
         <v>0</v>
       </c>
       <c r="T49">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U49">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V49">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W49">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X49">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y49">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z49">
         <v>0.65</v>
@@ -7542,22 +7555,22 @@
         <v>0</v>
       </c>
       <c r="T50">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U50">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V50">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W50">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X50">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y50">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z50">
         <v>0.65</v>
@@ -7682,22 +7695,22 @@
         <v>0</v>
       </c>
       <c r="T51">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U51">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V51">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W51">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X51">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y51">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z51">
         <v>0.65</v>
@@ -7822,22 +7835,22 @@
         <v>0</v>
       </c>
       <c r="T52">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U52">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V52">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W52">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X52">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y52">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z52">
         <v>0.65</v>
@@ -7962,37 +7975,37 @@
         <v>0</v>
       </c>
       <c r="T53">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U53">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V53">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W53">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X53">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y53">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z53">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AA53">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AB53">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AC53">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AD53">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AE53">
         <v>0.65</v>
@@ -8102,37 +8115,37 @@
         <v>0</v>
       </c>
       <c r="T54">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U54">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V54">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W54">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X54">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y54">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z54">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AA54">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AB54">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AC54">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AD54">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AE54">
         <v>0.65</v>
@@ -8242,37 +8255,37 @@
         <v>0</v>
       </c>
       <c r="T55">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U55">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V55">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W55">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X55">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y55">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z55">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AA55">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AB55">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AC55">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AD55">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AE55">
         <v>0.65</v>
@@ -8382,37 +8395,37 @@
         <v>0</v>
       </c>
       <c r="T56">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U56">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V56">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W56">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X56">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y56">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z56">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AA56">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AB56">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AC56">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AD56">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AE56">
         <v>0.65</v>
@@ -8522,37 +8535,37 @@
         <v>0</v>
       </c>
       <c r="T57">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U57">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V57">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W57">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X57">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y57">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z57">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AA57">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AB57">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AC57">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AD57">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AE57">
         <v>0.65</v>
@@ -8662,37 +8675,37 @@
         <v>0</v>
       </c>
       <c r="T58">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U58">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V58">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W58">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X58">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y58">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z58">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AA58">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AB58">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AC58">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AD58">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AE58">
         <v>0.65</v>
@@ -8802,37 +8815,37 @@
         <v>0</v>
       </c>
       <c r="T59">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U59">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V59">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W59">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X59">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y59">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z59">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AA59">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AB59">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AC59">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AD59">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AE59">
         <v>0.65</v>
@@ -8942,37 +8955,37 @@
         <v>0</v>
       </c>
       <c r="T60">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U60">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V60">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W60">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X60">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y60">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z60">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AA60">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AB60">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AC60">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AD60">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AE60">
         <v>0.65</v>
@@ -9082,37 +9095,37 @@
         <v>0</v>
       </c>
       <c r="T61">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U61">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V61">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W61">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X61">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y61">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z61">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AA61">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AB61">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AC61">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AD61">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AE61">
         <v>0.65</v>
@@ -9222,37 +9235,37 @@
         <v>0</v>
       </c>
       <c r="T62">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U62">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V62">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W62">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X62">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y62">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z62">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AA62">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AB62">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AC62">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AD62">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AE62">
         <v>0.65</v>
@@ -9362,37 +9375,37 @@
         <v>0</v>
       </c>
       <c r="T63">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U63">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V63">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W63">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X63">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y63">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z63">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AA63">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AB63">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AC63">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AD63">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AE63">
         <v>0.65</v>
@@ -9502,37 +9515,37 @@
         <v>0</v>
       </c>
       <c r="T64">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U64">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V64">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W64">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X64">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y64">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z64">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AA64">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AB64">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AC64">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AD64">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AE64">
         <v>0.65</v>
@@ -9642,37 +9655,37 @@
         <v>0</v>
       </c>
       <c r="T65">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U65">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V65">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W65">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X65">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y65">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z65">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AA65">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AB65">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AC65">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AD65">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AE65">
         <v>0.65</v>
@@ -9782,37 +9795,37 @@
         <v>0</v>
       </c>
       <c r="T66">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U66">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V66">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W66">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X66">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y66">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z66">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AA66">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AB66">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AC66">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AD66">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AE66">
         <v>0.65</v>
@@ -9922,37 +9935,37 @@
         <v>0</v>
       </c>
       <c r="T67">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U67">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V67">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W67">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X67">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y67">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z67">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AA67">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AB67">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AC67">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AD67">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AE67">
         <v>0.65</v>
@@ -10062,37 +10075,37 @@
         <v>0</v>
       </c>
       <c r="T68">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U68">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V68">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W68">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X68">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y68">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z68">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AA68">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AB68">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AC68">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AD68">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AE68">
         <v>0.65</v>
@@ -10202,37 +10215,37 @@
         <v>0</v>
       </c>
       <c r="T69">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="U69">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="V69">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="W69">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="X69">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Y69">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="Z69">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AA69">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AB69">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AC69">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AD69">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="AE69">
         <v>0.65</v>
@@ -10290,4 +10303,59 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>